<commit_message>
Updated Documentation,: Financial plan, House of Quality, Engineering Requirements
</commit_message>
<xml_diff>
--- a/Initial_Proposal_Parts/Project Timeline.xlsx
+++ b/Initial_Proposal_Parts/Project Timeline.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castr\Desktop\Senior Design 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castr\Documents\GitHub\Spring17-SeniorDesign\Initial_Proposal_Parts\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Fire Alarm" sheetId="3" r:id="rId1"/>
@@ -1035,10 +1035,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1049,9 +1045,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1084,6 +1077,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1398,9 +1398,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AS46"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="E42" sqref="A42:E46"/>
     </sheetView>
   </sheetViews>
@@ -1416,72 +1419,72 @@
       <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="85" t="s">
+      <c r="B1" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="84" t="s">
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84" t="s">
+      <c r="G1" s="126"/>
+      <c r="H1" s="126"/>
+      <c r="I1" s="126"/>
+      <c r="J1" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84" t="s">
+      <c r="K1" s="126"/>
+      <c r="L1" s="126"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84" t="s">
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84" t="s">
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84" t="s">
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84" t="s">
+      <c r="AA1" s="126"/>
+      <c r="AB1" s="126"/>
+      <c r="AC1" s="126"/>
+      <c r="AD1" s="126" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
-      <c r="AG1" s="84"/>
-      <c r="AH1" s="84" t="s">
+      <c r="AE1" s="126"/>
+      <c r="AF1" s="126"/>
+      <c r="AG1" s="126"/>
+      <c r="AH1" s="126" t="s">
         <v>10</v>
       </c>
-      <c r="AI1" s="84"/>
-      <c r="AJ1" s="84"/>
-      <c r="AK1" s="84"/>
-      <c r="AL1" s="84" t="s">
+      <c r="AI1" s="126"/>
+      <c r="AJ1" s="126"/>
+      <c r="AK1" s="126"/>
+      <c r="AL1" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="84"/>
-      <c r="AN1" s="84"/>
-      <c r="AO1" s="84"/>
-      <c r="AP1" s="84" t="s">
+      <c r="AM1" s="126"/>
+      <c r="AN1" s="126"/>
+      <c r="AO1" s="126"/>
+      <c r="AP1" s="126" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="84"/>
-      <c r="AR1" s="84"/>
-      <c r="AS1" s="87"/>
+      <c r="AQ1" s="126"/>
+      <c r="AR1" s="126"/>
+      <c r="AS1" s="127"/>
     </row>
     <row r="2" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
@@ -2030,9 +2033,9 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="13"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="117"/>
-      <c r="H13" s="117"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
       <c r="I13" s="11"/>
       <c r="J13" s="9"/>
       <c r="K13" s="10"/>
@@ -2626,25 +2629,25 @@
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="11"/>
-      <c r="N25" s="116"/>
-      <c r="O25" s="119"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="120"/>
-      <c r="R25" s="116"/>
-      <c r="S25" s="119"/>
-      <c r="T25" s="117"/>
-      <c r="U25" s="120"/>
-      <c r="V25" s="116"/>
-      <c r="W25" s="119"/>
-      <c r="X25" s="117"/>
-      <c r="Y25" s="120"/>
-      <c r="Z25" s="116"/>
-      <c r="AA25" s="119"/>
-      <c r="AB25" s="117"/>
-      <c r="AC25" s="120"/>
-      <c r="AD25" s="116"/>
-      <c r="AE25" s="119"/>
-      <c r="AF25" s="117"/>
+      <c r="N25" s="109"/>
+      <c r="O25" s="112"/>
+      <c r="P25" s="110"/>
+      <c r="Q25" s="113"/>
+      <c r="R25" s="109"/>
+      <c r="S25" s="112"/>
+      <c r="T25" s="110"/>
+      <c r="U25" s="113"/>
+      <c r="V25" s="109"/>
+      <c r="W25" s="112"/>
+      <c r="X25" s="110"/>
+      <c r="Y25" s="113"/>
+      <c r="Z25" s="109"/>
+      <c r="AA25" s="112"/>
+      <c r="AB25" s="110"/>
+      <c r="AC25" s="113"/>
+      <c r="AD25" s="109"/>
+      <c r="AE25" s="112"/>
+      <c r="AF25" s="110"/>
       <c r="AG25" s="11"/>
       <c r="AH25" s="9"/>
       <c r="AI25" s="10"/>
@@ -3035,12 +3038,12 @@
       <c r="Z33" s="9"/>
       <c r="AA33" s="10"/>
       <c r="AB33" s="10"/>
-      <c r="AC33" s="115"/>
-      <c r="AD33" s="118"/>
-      <c r="AE33" s="117"/>
-      <c r="AF33" s="119"/>
-      <c r="AG33" s="115"/>
-      <c r="AH33" s="118"/>
+      <c r="AC33" s="108"/>
+      <c r="AD33" s="111"/>
+      <c r="AE33" s="110"/>
+      <c r="AF33" s="112"/>
+      <c r="AG33" s="108"/>
+      <c r="AH33" s="111"/>
       <c r="AI33" s="10"/>
       <c r="AJ33" s="10"/>
       <c r="AK33" s="11"/>
@@ -3415,7 +3418,7 @@
       <c r="B43" s="51"/>
       <c r="C43" s="51"/>
       <c r="D43" s="51"/>
-      <c r="E43" s="132"/>
+      <c r="E43" s="125"/>
     </row>
     <row r="44" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A44" s="83" t="s">
@@ -3427,47 +3430,50 @@
       <c r="E44" s="81"/>
     </row>
     <row r="45" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A45" s="112" t="s">
+      <c r="A45" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="130"/>
-      <c r="C45" s="130"/>
-      <c r="D45" s="130"/>
-      <c r="E45" s="131"/>
+      <c r="B45" s="123"/>
+      <c r="C45" s="123"/>
+      <c r="D45" s="123"/>
+      <c r="E45" s="124"/>
     </row>
     <row r="46" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="114" t="s">
+      <c r="A46" s="107" t="s">
         <v>87</v>
       </c>
       <c r="B46" s="69"/>
       <c r="C46" s="69"/>
       <c r="D46" s="69"/>
-      <c r="E46" s="113"/>
+      <c r="E46" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="R1:U1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="74" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AS48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A44" sqref="A44:E48"/>
     </sheetView>
   </sheetViews>
@@ -3480,75 +3486,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98" t="s">
+      <c r="C1" s="130"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98" t="s">
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98" t="s">
+      <c r="K1" s="130"/>
+      <c r="L1" s="130"/>
+      <c r="M1" s="130"/>
+      <c r="N1" s="130" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98" t="s">
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="99" t="s">
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="98"/>
-      <c r="X1" s="98"/>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="98" t="s">
+      <c r="W1" s="130"/>
+      <c r="X1" s="130"/>
+      <c r="Y1" s="130"/>
+      <c r="Z1" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="AA1" s="98"/>
-      <c r="AB1" s="98"/>
-      <c r="AC1" s="98"/>
-      <c r="AD1" s="99" t="s">
+      <c r="AA1" s="130"/>
+      <c r="AB1" s="130"/>
+      <c r="AC1" s="130"/>
+      <c r="AD1" s="131" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="98"/>
-      <c r="AF1" s="98"/>
-      <c r="AG1" s="98"/>
-      <c r="AH1" s="98" t="s">
+      <c r="AE1" s="130"/>
+      <c r="AF1" s="130"/>
+      <c r="AG1" s="130"/>
+      <c r="AH1" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="AI1" s="98"/>
-      <c r="AJ1" s="98"/>
-      <c r="AK1" s="98"/>
-      <c r="AL1" s="99" t="s">
+      <c r="AI1" s="130"/>
+      <c r="AJ1" s="130"/>
+      <c r="AK1" s="130"/>
+      <c r="AL1" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="AM1" s="98"/>
-      <c r="AN1" s="98"/>
-      <c r="AO1" s="98"/>
-      <c r="AP1" s="98" t="s">
+      <c r="AM1" s="130"/>
+      <c r="AN1" s="130"/>
+      <c r="AO1" s="130"/>
+      <c r="AP1" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="AQ1" s="98"/>
-      <c r="AR1" s="98"/>
-      <c r="AS1" s="100"/>
+      <c r="AQ1" s="130"/>
+      <c r="AR1" s="130"/>
+      <c r="AS1" s="132"/>
     </row>
     <row r="2" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="30" t="s">
@@ -3600,14 +3606,14 @@
       <c r="AS2" s="34"/>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A3" s="101" t="s">
+      <c r="A3" s="94" t="s">
         <v>56</v>
       </c>
       <c r="B3" s="74"/>
       <c r="C3" s="75"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="88"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="5"/>
@@ -3698,14 +3704,14 @@
       <c r="AS4" s="20"/>
     </row>
     <row r="5" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A5" s="101" t="s">
+      <c r="A5" s="94" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="90"/>
-      <c r="F5" s="88"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="119"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="5"/>
@@ -3796,14 +3802,14 @@
       <c r="AS6" s="20"/>
     </row>
     <row r="7" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A7" s="101" t="s">
+      <c r="A7" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="128"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="126"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="88"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="119"/>
+      <c r="D7" s="119"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="84"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="5"/>
@@ -3845,7 +3851,7 @@
       <c r="AS7" s="22"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A8" s="102" t="s">
+      <c r="A8" s="95" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="48"/>
@@ -3894,14 +3900,14 @@
       <c r="AS8" s="20"/>
     </row>
     <row r="9" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A9" s="103" t="s">
+      <c r="A9" s="96" t="s">
         <v>63</v>
       </c>
       <c r="B9" s="74"/>
       <c r="C9" s="75"/>
       <c r="D9" s="75"/>
-      <c r="E9" s="90"/>
-      <c r="F9" s="88"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="84"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="5"/>
@@ -3992,13 +3998,13 @@
       <c r="AS10" s="20"/>
     </row>
     <row r="11" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A11" s="102" t="s">
+      <c r="A11" s="95" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="75"/>
-      <c r="E11" s="122"/>
+      <c r="E11" s="115"/>
       <c r="F11" s="74"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
@@ -4090,14 +4096,14 @@
       <c r="AS12" s="20"/>
     </row>
     <row r="13" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="95" t="s">
         <v>75</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="73"/>
       <c r="E13" s="72"/>
-      <c r="F13" s="121"/>
+      <c r="F13" s="114"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="5"/>
@@ -4188,16 +4194,16 @@
       <c r="AS14" s="34"/>
     </row>
     <row r="15" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A15" s="101" t="s">
+      <c r="A15" s="94" t="s">
         <v>65</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
-      <c r="F15" s="128"/>
-      <c r="G15" s="126"/>
-      <c r="H15" s="126"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
       <c r="I15" s="5"/>
       <c r="J15" s="3"/>
       <c r="K15" s="4"/>
@@ -4237,7 +4243,7 @@
       <c r="AS15" s="22"/>
     </row>
     <row r="16" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="96" t="s">
         <v>66</v>
       </c>
       <c r="B16" s="2"/>
@@ -4286,16 +4292,16 @@
       <c r="AS16" s="20"/>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A17" s="101" t="s">
+      <c r="A17" s="94" t="s">
         <v>74</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="123"/>
-      <c r="G17" s="124"/>
-      <c r="H17" s="124"/>
+      <c r="F17" s="116"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="117"/>
       <c r="I17" s="5"/>
       <c r="J17" s="3"/>
       <c r="K17" s="4"/>
@@ -4335,7 +4341,7 @@
       <c r="AS17" s="22"/>
     </row>
     <row r="18" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A18" s="103" t="s">
+      <c r="A18" s="96" t="s">
         <v>67</v>
       </c>
       <c r="B18" s="2"/>
@@ -4384,7 +4390,7 @@
       <c r="AS18" s="20"/>
     </row>
     <row r="19" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="94" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="3"/>
@@ -4393,9 +4399,9 @@
       <c r="E19" s="5"/>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="124"/>
-      <c r="I19" s="125"/>
-      <c r="J19" s="123"/>
+      <c r="H19" s="117"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="116"/>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
       <c r="M19" s="5"/>
@@ -4433,7 +4439,7 @@
       <c r="AS19" s="22"/>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
+      <c r="A20" s="96" t="s">
         <v>69</v>
       </c>
       <c r="B20" s="2"/>
@@ -4482,7 +4488,7 @@
       <c r="AS20" s="20"/>
     </row>
     <row r="21" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A21" s="101" t="s">
+      <c r="A21" s="94" t="s">
         <v>70</v>
       </c>
       <c r="B21" s="3"/>
@@ -4491,9 +4497,9 @@
       <c r="E21" s="5"/>
       <c r="F21" s="3"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="126"/>
-      <c r="I21" s="127"/>
-      <c r="J21" s="128"/>
+      <c r="H21" s="119"/>
+      <c r="I21" s="120"/>
+      <c r="J21" s="121"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="5"/>
@@ -4531,7 +4537,7 @@
       <c r="AS21" s="22"/>
     </row>
     <row r="22" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A22" s="103" t="s">
+      <c r="A22" s="96" t="s">
         <v>71</v>
       </c>
       <c r="B22" s="2"/>
@@ -4589,11 +4595,11 @@
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="91"/>
+      <c r="H23" s="87"/>
       <c r="I23" s="46"/>
-      <c r="J23" s="129"/>
-      <c r="K23" s="130"/>
-      <c r="L23" s="130"/>
+      <c r="J23" s="122"/>
+      <c r="K23" s="123"/>
+      <c r="L23" s="123"/>
       <c r="M23" s="7"/>
       <c r="N23" s="8"/>
       <c r="O23" s="6"/>
@@ -4629,7 +4635,7 @@
       <c r="AS23" s="29"/>
     </row>
     <row r="24" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A24" s="103" t="s">
+      <c r="A24" s="96" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="2"/>
@@ -4640,10 +4646,10 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="121"/>
+      <c r="J24" s="114"/>
       <c r="K24" s="75"/>
       <c r="L24" s="73"/>
-      <c r="M24" s="122"/>
+      <c r="M24" s="115"/>
       <c r="N24" s="2"/>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
@@ -4678,7 +4684,7 @@
       <c r="AS24" s="20"/>
     </row>
     <row r="25" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101" t="s">
+      <c r="A25" s="94" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="3"/>
@@ -4689,10 +4695,10 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="123"/>
-      <c r="K25" s="126"/>
-      <c r="L25" s="124"/>
-      <c r="M25" s="127"/>
+      <c r="J25" s="116"/>
+      <c r="K25" s="119"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="120"/>
       <c r="N25" s="3"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -4776,7 +4782,7 @@
       <c r="AS26" s="34"/>
     </row>
     <row r="27" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A27" s="106" t="s">
+      <c r="A27" s="99" t="s">
         <v>73</v>
       </c>
       <c r="B27" s="3"/>
@@ -4791,26 +4797,26 @@
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
       <c r="M27" s="5"/>
-      <c r="N27" s="123"/>
-      <c r="O27" s="126"/>
-      <c r="P27" s="124"/>
-      <c r="Q27" s="127"/>
-      <c r="R27" s="123"/>
-      <c r="S27" s="126"/>
-      <c r="T27" s="124"/>
-      <c r="U27" s="127"/>
-      <c r="V27" s="123"/>
-      <c r="W27" s="126"/>
-      <c r="X27" s="124"/>
-      <c r="Y27" s="127"/>
-      <c r="Z27" s="123"/>
-      <c r="AA27" s="126"/>
-      <c r="AB27" s="124"/>
-      <c r="AC27" s="127"/>
-      <c r="AD27" s="123"/>
-      <c r="AE27" s="126"/>
-      <c r="AF27" s="124"/>
-      <c r="AG27" s="90"/>
+      <c r="N27" s="116"/>
+      <c r="O27" s="119"/>
+      <c r="P27" s="117"/>
+      <c r="Q27" s="120"/>
+      <c r="R27" s="116"/>
+      <c r="S27" s="119"/>
+      <c r="T27" s="117"/>
+      <c r="U27" s="120"/>
+      <c r="V27" s="116"/>
+      <c r="W27" s="119"/>
+      <c r="X27" s="117"/>
+      <c r="Y27" s="120"/>
+      <c r="Z27" s="116"/>
+      <c r="AA27" s="119"/>
+      <c r="AB27" s="117"/>
+      <c r="AC27" s="120"/>
+      <c r="AD27" s="116"/>
+      <c r="AE27" s="119"/>
+      <c r="AF27" s="117"/>
+      <c r="AG27" s="86"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="4"/>
       <c r="AJ27" s="4"/>
@@ -4825,7 +4831,7 @@
       <c r="AS27" s="22"/>
     </row>
     <row r="28" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="98" t="s">
         <v>76</v>
       </c>
       <c r="B28" s="2"/>
@@ -4874,7 +4880,7 @@
       <c r="AS28" s="20"/>
     </row>
     <row r="29" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A29" s="104" t="s">
+      <c r="A29" s="97" t="s">
         <v>66</v>
       </c>
       <c r="B29" s="3"/>
@@ -4889,11 +4895,11 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="5"/>
-      <c r="N29" s="121"/>
+      <c r="N29" s="114"/>
       <c r="O29" s="73"/>
       <c r="P29" s="73"/>
       <c r="Q29" s="72"/>
-      <c r="R29" s="121"/>
+      <c r="R29" s="114"/>
       <c r="S29" s="73"/>
       <c r="T29" s="73"/>
       <c r="U29" s="72"/>
@@ -4901,7 +4907,7 @@
       <c r="W29" s="73"/>
       <c r="X29" s="73"/>
       <c r="Y29" s="73"/>
-      <c r="Z29" s="121"/>
+      <c r="Z29" s="114"/>
       <c r="AA29" s="73"/>
       <c r="AB29" s="73"/>
       <c r="AC29" s="72"/>
@@ -4923,7 +4929,7 @@
       <c r="AS29" s="22"/>
     </row>
     <row r="30" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A30" s="105" t="s">
+      <c r="A30" s="98" t="s">
         <v>67</v>
       </c>
       <c r="B30" s="2"/>
@@ -4972,7 +4978,7 @@
       <c r="AS30" s="20"/>
     </row>
     <row r="31" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A31" s="104" t="s">
+      <c r="A31" s="97" t="s">
         <v>77</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -4992,11 +4998,11 @@
       <c r="N31" s="74"/>
       <c r="O31" s="75"/>
       <c r="P31" s="75"/>
-      <c r="Q31" s="122"/>
+      <c r="Q31" s="115"/>
       <c r="R31" s="74"/>
       <c r="S31" s="75"/>
       <c r="T31" s="75"/>
-      <c r="U31" s="122"/>
+      <c r="U31" s="115"/>
       <c r="V31" s="75"/>
       <c r="W31" s="75"/>
       <c r="X31" s="75"/>
@@ -5004,7 +5010,7 @@
       <c r="Z31" s="74"/>
       <c r="AA31" s="75"/>
       <c r="AB31" s="75"/>
-      <c r="AC31" s="122"/>
+      <c r="AC31" s="115"/>
       <c r="AD31" s="75"/>
       <c r="AE31" s="75"/>
       <c r="AF31" s="75"/>
@@ -5023,7 +5029,7 @@
       <c r="AS31" s="22"/>
     </row>
     <row r="32" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="98" t="s">
         <v>78</v>
       </c>
       <c r="B32" s="2"/>
@@ -5072,7 +5078,7 @@
       <c r="AS32" s="20"/>
     </row>
     <row r="33" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="97" t="s">
         <v>75</v>
       </c>
       <c r="B33" s="3"/>
@@ -5087,26 +5093,26 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="5"/>
-      <c r="N33" s="121"/>
+      <c r="N33" s="114"/>
       <c r="O33" s="75"/>
       <c r="P33" s="73"/>
-      <c r="Q33" s="122"/>
-      <c r="R33" s="121"/>
+      <c r="Q33" s="115"/>
+      <c r="R33" s="114"/>
       <c r="S33" s="75"/>
       <c r="T33" s="73"/>
-      <c r="U33" s="122"/>
-      <c r="V33" s="121"/>
+      <c r="U33" s="115"/>
+      <c r="V33" s="114"/>
       <c r="W33" s="75"/>
       <c r="X33" s="73"/>
-      <c r="Y33" s="122"/>
-      <c r="Z33" s="121"/>
+      <c r="Y33" s="115"/>
+      <c r="Z33" s="114"/>
       <c r="AA33" s="75"/>
       <c r="AB33" s="73"/>
-      <c r="AC33" s="122"/>
-      <c r="AD33" s="121"/>
+      <c r="AC33" s="115"/>
+      <c r="AD33" s="114"/>
       <c r="AE33" s="75"/>
       <c r="AF33" s="73"/>
-      <c r="AG33" s="122"/>
+      <c r="AG33" s="115"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="4"/>
       <c r="AJ33" s="4"/>
@@ -5170,42 +5176,42 @@
       <c r="AS34" s="34"/>
     </row>
     <row r="35" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A35" s="111" t="s">
+      <c r="A35" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="107"/>
-      <c r="C35" s="108"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="109"/>
-      <c r="F35" s="107"/>
-      <c r="G35" s="108"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="107"/>
-      <c r="K35" s="108"/>
-      <c r="L35" s="108"/>
-      <c r="M35" s="109"/>
-      <c r="N35" s="107"/>
-      <c r="O35" s="108"/>
-      <c r="P35" s="108"/>
-      <c r="Q35" s="109"/>
-      <c r="R35" s="107"/>
-      <c r="S35" s="108"/>
-      <c r="T35" s="108"/>
-      <c r="U35" s="109"/>
-      <c r="V35" s="108"/>
-      <c r="W35" s="108"/>
-      <c r="X35" s="108"/>
-      <c r="Y35" s="108"/>
-      <c r="Z35" s="107"/>
-      <c r="AA35" s="108"/>
-      <c r="AB35" s="108"/>
-      <c r="AC35" s="115"/>
-      <c r="AD35" s="118"/>
-      <c r="AE35" s="117"/>
-      <c r="AF35" s="119"/>
-      <c r="AG35" s="115"/>
-      <c r="AH35" s="118"/>
+      <c r="B35" s="100"/>
+      <c r="C35" s="101"/>
+      <c r="D35" s="101"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="101"/>
+      <c r="H35" s="101"/>
+      <c r="I35" s="102"/>
+      <c r="J35" s="100"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="101"/>
+      <c r="M35" s="102"/>
+      <c r="N35" s="100"/>
+      <c r="O35" s="101"/>
+      <c r="P35" s="101"/>
+      <c r="Q35" s="102"/>
+      <c r="R35" s="100"/>
+      <c r="S35" s="101"/>
+      <c r="T35" s="101"/>
+      <c r="U35" s="102"/>
+      <c r="V35" s="101"/>
+      <c r="W35" s="101"/>
+      <c r="X35" s="101"/>
+      <c r="Y35" s="101"/>
+      <c r="Z35" s="100"/>
+      <c r="AA35" s="101"/>
+      <c r="AB35" s="101"/>
+      <c r="AC35" s="108"/>
+      <c r="AD35" s="111"/>
+      <c r="AE35" s="110"/>
+      <c r="AF35" s="112"/>
+      <c r="AG35" s="108"/>
+      <c r="AH35" s="111"/>
       <c r="AI35" s="10"/>
       <c r="AJ35" s="10"/>
       <c r="AK35" s="11"/>
@@ -5214,9 +5220,9 @@
       <c r="AN35" s="10"/>
       <c r="AO35" s="11"/>
       <c r="AP35" s="9"/>
-      <c r="AQ35" s="108"/>
-      <c r="AR35" s="108"/>
-      <c r="AS35" s="110"/>
+      <c r="AQ35" s="101"/>
+      <c r="AR35" s="101"/>
+      <c r="AS35" s="103"/>
     </row>
     <row r="36" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
@@ -5403,7 +5409,7 @@
       <c r="AG39" s="76"/>
       <c r="AH39" s="77"/>
       <c r="AI39" s="78"/>
-      <c r="AJ39" s="89"/>
+      <c r="AJ39" s="85"/>
       <c r="AK39" s="5"/>
       <c r="AL39" s="3"/>
       <c r="AM39" s="4"/>
@@ -5513,36 +5519,36 @@
       <c r="AS41" s="20"/>
     </row>
     <row r="42" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="92" t="s">
+      <c r="A42" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="93"/>
-      <c r="C42" s="94"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="93"/>
-      <c r="G42" s="94"/>
-      <c r="H42" s="94"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="94"/>
-      <c r="L42" s="94"/>
-      <c r="M42" s="95"/>
-      <c r="N42" s="93"/>
-      <c r="O42" s="94"/>
-      <c r="P42" s="94"/>
-      <c r="Q42" s="95"/>
-      <c r="R42" s="93"/>
-      <c r="S42" s="94"/>
-      <c r="T42" s="94"/>
-      <c r="U42" s="95"/>
-      <c r="V42" s="94"/>
-      <c r="W42" s="94"/>
-      <c r="X42" s="94"/>
-      <c r="Y42" s="94"/>
-      <c r="Z42" s="93"/>
-      <c r="AA42" s="94"/>
-      <c r="AB42" s="94"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="90"/>
+      <c r="D42" s="90"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="89"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="91"/>
+      <c r="N42" s="89"/>
+      <c r="O42" s="90"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="91"/>
+      <c r="R42" s="89"/>
+      <c r="S42" s="90"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="91"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+      <c r="X42" s="90"/>
+      <c r="Y42" s="90"/>
+      <c r="Z42" s="89"/>
+      <c r="AA42" s="90"/>
+      <c r="AB42" s="90"/>
       <c r="AC42" s="27"/>
       <c r="AD42" s="25"/>
       <c r="AE42" s="26"/>
@@ -5557,9 +5563,9 @@
       <c r="AN42" s="69"/>
       <c r="AO42" s="70"/>
       <c r="AP42" s="71"/>
-      <c r="AQ42" s="94"/>
-      <c r="AR42" s="94"/>
-      <c r="AS42" s="96"/>
+      <c r="AQ42" s="90"/>
+      <c r="AR42" s="90"/>
+      <c r="AS42" s="92"/>
     </row>
     <row r="43" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
@@ -5580,7 +5586,7 @@
       <c r="B45" s="51"/>
       <c r="C45" s="51"/>
       <c r="D45" s="51"/>
-      <c r="E45" s="132"/>
+      <c r="E45" s="125"/>
     </row>
     <row r="46" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A46" s="83" t="s">
@@ -5592,38 +5598,38 @@
       <c r="E46" s="81"/>
     </row>
     <row r="47" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A47" s="112" t="s">
+      <c r="A47" s="105" t="s">
         <v>55</v>
       </c>
-      <c r="B47" s="130"/>
-      <c r="C47" s="130"/>
-      <c r="D47" s="130"/>
-      <c r="E47" s="131"/>
+      <c r="B47" s="123"/>
+      <c r="C47" s="123"/>
+      <c r="D47" s="123"/>
+      <c r="E47" s="124"/>
     </row>
     <row r="48" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="114" t="s">
+      <c r="A48" s="107" t="s">
         <v>87</v>
       </c>
       <c r="B48" s="69"/>
       <c r="C48" s="69"/>
       <c r="D48" s="69"/>
-      <c r="E48" s="113"/>
+      <c r="E48" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AS1"/>
     <mergeCell ref="V1:Y1"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="R1:U1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AS1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="71" fitToWidth="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>